<commit_message>
fix pickerInput issue when deploying
issues fixed using deprecated version of shiny and bslib
</commit_message>
<xml_diff>
--- a/ncaa_pitching_data_status.xlsx
+++ b/ncaa_pitching_data_status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewadams/Documents/R Projects/Baseball Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888F7E58-710A-BD40-9ABE-8CB9BC2D91B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142C22A6-62A9-2B46-8C00-DA67549F2672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="10000" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="19820" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
   <si>
     <t>team</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>UCSB</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>not-pulled</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -766,45 +772,80 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>